<commit_message>
Fixed Spielerranglisten Changed Spielerranglisten and FileCreators Fixed search-function Added Club-Images to Clubs Improved Calendar on Startpage Added 3 new categories to all pages required Added more infos to calendar-popups Fixed Froala-Bug Fixed Froala Fileuploader plugin
</commit_message>
<xml_diff>
--- a/files/spielerranglisten/Spielerrangliste-2017-2018-alle.xlsx
+++ b/files/spielerranglisten/Spielerrangliste-2017-2018-alle.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>OÖBV - Mannschaftsmeisterschaft</t>
   </si>
@@ -29,53 +29,7 @@
     <t>S P I E L E R R A N G L I S T E</t>
   </si>
   <si>
-    <t>Stand per 09.02.2018</t>
-  </si>
-  <si>
-    <t>Union VKB  Braunau</t>
-  </si>
-  <si>
-    <t>Änderungen/
-Mannschaftsf.</t>
-  </si>
-  <si>
-    <t>Handy-Nr.</t>
-  </si>
-  <si>
-    <t>E-Mail</t>
-  </si>
-  <si>
-    <t>Nachname</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Mitgl. Nr.</t>
-  </si>
-  <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>Vereins-Nr.</t>
-  </si>
-  <si>
-    <t>Herren</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>Jauch</t>
-  </si>
-  <si>
-    <t>Günter</t>
-  </si>
-  <si>
-    <t>Hallo</t>
-  </si>
-  <si>
-    <t>Damen</t>
+    <t>Stand per 01.01.1970</t>
   </si>
 </sst>
 </file>
@@ -86,15 +40,6 @@
   <fonts count="5">
     <font>
       <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -129,8 +74,17 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,19 +96,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1E90FF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF32CD32"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF1E90FF"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -165,60 +113,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="10">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="4" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="4" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,10 +478,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -574,182 +498,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customHeight="1" ht="40.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" customHeight="1" ht="21">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="7"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" customHeight="1" ht="24">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="7"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="8" spans="1:9" customHeight="1" ht="30">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12">
-        <v>310</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" customHeight="1" ht="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1">
-        <v>200</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
-        <v>310</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="15"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="6"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -758,7 +580,6 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:I3"/>
-    <mergeCell ref="A8:E8"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>